<commit_message>
improve 2017 Day 1
</commit_message>
<xml_diff>
--- a/2022/Day04.xlsx
+++ b/2022/Day04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfalero/Documents/Excel/Excel &amp; Financial Modelling/Advent-of-Code-Excel/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFE413A-20CA-FA43-A980-8AE139979D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79203CEB-0E17-1949-8ACF-C9D7A58CF825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40960" yWindow="500" windowWidth="24740" windowHeight="16360" activeTab="2" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33620" windowHeight="21580" activeTab="2" xr2:uid="{BD9D965C-81AA-E441-BA42-DB93D2E4F26D}"/>
   </bookViews>
   <sheets>
     <sheet name="Solutions" sheetId="3" r:id="rId1"/>
@@ -29,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -41497,12 +41499,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A99312-316D-ED49-896B-A365DEB058D4}">
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="12" width="11" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>